<commit_message>
marked common concepts in both ontologies, total has 28 terms
</commit_message>
<xml_diff>
--- a/src/ontology/obcs_terms.xlsx
+++ b/src/ontology/obcs_terms.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="24795" windowHeight="12270"/>
+    <workbookView xWindow="12600" yWindow="-15" windowWidth="12645" windowHeight="12480"/>
   </bookViews>
   <sheets>
     <sheet name="obcs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="453">
   <si>
     <t>Name</t>
   </si>
@@ -1370,6 +1370,9 @@
   </si>
   <si>
     <t>validity</t>
+  </si>
+  <si>
+    <t>28 terms in common</t>
   </si>
 </sst>
 </file>
@@ -1862,9 +1865,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2200,10 +2205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D138"/>
+  <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2284,7 +2289,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B7" t="s">
@@ -2353,7 +2358,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>385</v>
       </c>
       <c r="B13" t="s">
@@ -2375,7 +2380,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>259</v>
       </c>
       <c r="B15" t="s">
@@ -2450,7 +2455,7 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>225</v>
       </c>
       <c r="B21" t="s">
@@ -2475,7 +2480,7 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>213</v>
       </c>
       <c r="B23" t="s">
@@ -2486,7 +2491,7 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>432</v>
       </c>
       <c r="B24" t="s">
@@ -2737,7 +2742,7 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>267</v>
       </c>
       <c r="B46" t="s">
@@ -2759,7 +2764,7 @@
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B48" t="s">
@@ -2773,7 +2778,7 @@
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>331</v>
       </c>
       <c r="B49" t="s">
@@ -2806,7 +2811,7 @@
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B52" t="s">
@@ -2817,7 +2822,7 @@
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" t="s">
+      <c r="A53" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B53" t="s">
@@ -2964,7 +2969,7 @@
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" t="s">
+      <c r="A65" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B65" t="s">
@@ -2986,7 +2991,7 @@
       </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" t="s">
+      <c r="A67" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B67" t="s">
@@ -3058,7 +3063,7 @@
       </c>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" t="s">
+      <c r="A73" s="2" t="s">
         <v>334</v>
       </c>
       <c r="B73" t="s">
@@ -3130,7 +3135,7 @@
       </c>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" t="s">
+      <c r="A79" s="2" t="s">
         <v>372</v>
       </c>
       <c r="B79" t="s">
@@ -3141,7 +3146,7 @@
       </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" t="s">
+      <c r="A80" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B80" t="s">
@@ -3263,7 +3268,7 @@
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" t="s">
+      <c r="A90" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B90" t="s">
@@ -3285,7 +3290,7 @@
       </c>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" t="s">
+      <c r="A92" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B92" t="s">
@@ -3354,7 +3359,7 @@
       </c>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" t="s">
+      <c r="A98" s="2" t="s">
         <v>150</v>
       </c>
       <c r="B98" t="s">
@@ -3437,7 +3442,7 @@
       </c>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" t="s">
+      <c r="A105" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B105" t="s">
@@ -3448,7 +3453,7 @@
       </c>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" t="s">
+      <c r="A106" s="2" t="s">
         <v>317</v>
       </c>
       <c r="B106" t="s">
@@ -3481,7 +3486,7 @@
       </c>
     </row>
     <row r="109" spans="1:4">
-      <c r="A109" t="s">
+      <c r="A109" s="2" t="s">
         <v>407</v>
       </c>
       <c r="B109" t="s">
@@ -3517,7 +3522,7 @@
       </c>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" t="s">
+      <c r="A112" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B112" t="s">
@@ -3572,7 +3577,7 @@
       </c>
     </row>
     <row r="117" spans="1:4">
-      <c r="A117" t="s">
+      <c r="A117" s="2" t="s">
         <v>449</v>
       </c>
       <c r="B117" t="s">
@@ -3586,7 +3591,7 @@
       </c>
     </row>
     <row r="118" spans="1:4">
-      <c r="A118" t="s">
+      <c r="A118" s="2" t="s">
         <v>450</v>
       </c>
       <c r="B118" t="s">
@@ -3600,7 +3605,7 @@
       </c>
     </row>
     <row r="119" spans="1:4">
-      <c r="A119" t="s">
+      <c r="A119" s="2" t="s">
         <v>245</v>
       </c>
       <c r="B119" t="s">
@@ -3669,7 +3674,7 @@
       </c>
     </row>
     <row r="125" spans="1:4">
-      <c r="A125" t="s">
+      <c r="A125" s="2" t="s">
         <v>263</v>
       </c>
       <c r="B125" t="s">
@@ -3722,7 +3727,7 @@
       </c>
     </row>
     <row r="129" spans="1:4">
-      <c r="A129" t="s">
+      <c r="A129" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B129" t="s">
@@ -3747,7 +3752,7 @@
       </c>
     </row>
     <row r="131" spans="1:4">
-      <c r="A131" t="s">
+      <c r="A131" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B131" t="s">
@@ -3761,7 +3766,7 @@
       </c>
     </row>
     <row r="132" spans="1:4">
-      <c r="A132" t="s">
+      <c r="A132" s="3" t="s">
         <v>252</v>
       </c>
       <c r="B132" t="s">
@@ -3844,6 +3849,11 @@
       </c>
       <c r="D138" t="s">
         <v>367</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" t="s">
+        <v>452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>